<commit_message>
update script and excel sheet
</commit_message>
<xml_diff>
--- a/MITKY-CustomEventLogEventIDs.xlsx
+++ b/MITKY-CustomEventLogEventIDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitky0051-my.sharepoint.com/personal/jason_mitky_com/Documents/Documents/GitHub/RMMCustomMonitors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="273" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C777CCD1-05D8-442D-8DF0-1736B96CDA89}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{946702BB-B71F-4FA8-9761-8F11E6EE5614}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{207F7709-C117-4E36-9CC8-F108324BDCB9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>EVENT ID</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Failed to rotate divisions! Check if any revisions are open in another process.</t>
+  </si>
+  <si>
+    <t>There were less than four backup revisions. An additional revision was scheduled.</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -359,9 +362,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,6 +369,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,6 +730,41 @@
             </a:rPr>
             <a:t>Use XXX9 for optimal results.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use subsequent</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> numbers for additional information.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -1818,19 +1859,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1873,11 +1914,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -2274,11 +2315,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -2444,10 +2485,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07352D7-56BB-4359-8F7E-BF3E06B00285}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,11 +2503,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
@@ -2565,18 +2606,32 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+    <row r="8" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
         <v>8109</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="29" t="s">
+      <c r="B8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="32" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>8110</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update organization and sheet
</commit_message>
<xml_diff>
--- a/MITKY-CustomEventLogEventIDs.xlsx
+++ b/MITKY-CustomEventLogEventIDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitky0051-my.sharepoint.com/personal/jason_mitky_com/Documents/Documents/GitHub/RMMCustomMonitors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="356" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A39CD81A-E59C-492B-AB64-732B44A403B2}"/>
+  <xr:revisionPtr revIDLastSave="520" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3B645D3-7041-4AE1-95E3-3007B171A466}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{207F7709-C117-4E36-9CC8-F108324BDCB9}"/>
   </bookViews>
@@ -16,8 +16,9 @@
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="Deployment Events" sheetId="6" r:id="rId2"/>
     <sheet name="Host Monitoring Events" sheetId="1" r:id="rId3"/>
-    <sheet name="VM Monitoring Events" sheetId="3" r:id="rId4"/>
-    <sheet name="Maintenance Task Events" sheetId="4" r:id="rId5"/>
+    <sheet name="WSB Events" sheetId="9" r:id="rId4"/>
+    <sheet name="VM Monitoring Events" sheetId="3" r:id="rId5"/>
+    <sheet name="Maintenance Task Events" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
   <si>
     <t>EVENT ID</t>
   </si>
@@ -111,15 +112,9 @@
     <t>External backups are scheduled, but the external backup drive was not found!</t>
   </si>
   <si>
-    <t>Windows Server Backup goes directly to the external backup drive. Consider installing an additional drive.</t>
-  </si>
-  <si>
     <t>External backups are scheduled, but no revisions are present.</t>
   </si>
   <si>
-    <t>External backups are scheduled, but the latest revision on the drive is out of date.</t>
-  </si>
-  <si>
     <t>At least one recent backup revision is present on the external drive.</t>
   </si>
   <si>
@@ -144,9 +139,6 @@
     <t>Backup revisions could not be checked because of recent backup failures.</t>
   </si>
   <si>
-    <t>No external backup drive was found. External backups are not scheduled.</t>
-  </si>
-  <si>
     <t>No Virtual Machines were detected or the Get-VM cmdlet failed! Check if Hyper-V is enabled for this server or if VMs should be present.</t>
   </si>
   <si>
@@ -177,9 +169,6 @@
     <t>There were less than four backup revisions. An additional revision was scheduled.</t>
   </si>
   <si>
-    <t>Maintenance Tasks</t>
-  </si>
-  <si>
     <t>(DO NOT USE) Deleting shadow copies critical event.</t>
   </si>
   <si>
@@ -201,13 +190,22 @@
     <t>Task $newTaskName was created or updated successfully.</t>
   </si>
   <si>
-    <t>Shadow copies were found on host server and could not be cleared!</t>
-  </si>
-  <si>
-    <t>Shadow copies were found on host server and successfully cleared.</t>
-  </si>
-  <si>
-    <t>No shadow copies were found on host server.</t>
+    <t>WINDOWS SERVER BACKUP EVENTS</t>
+  </si>
+  <si>
+    <t>No external backup drive was found! External backups are not scheduled.</t>
+  </si>
+  <si>
+    <t>The last Windows Server Backup was not successful! No revisions were changed on the external backup drive.</t>
+  </si>
+  <si>
+    <t>Windows Server Backup goes directly to the external backup drive! Consider installing an internal backup drive.</t>
+  </si>
+  <si>
+    <t>The last external backup revision could not be renamed! Check if another process has the folder or files open.</t>
+  </si>
+  <si>
+    <t>Failed to rotate external backup divisions! Check if any revisions are open in another process.</t>
   </si>
 </sst>
 </file>
@@ -292,31 +290,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +301,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,25 +360,14 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,89 +376,128 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -481,6 +507,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD85B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -501,7 +532,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5467350" cy="4352925"/>
+    <xdr:ext cx="5467350" cy="5295900"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -516,7 +547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19050" y="285750"/>
-          <a:ext cx="5467350" cy="4352925"/>
+          <a:ext cx="5467350" cy="5295900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -591,6 +622,70 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Scheduled Tasks</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Use this for scheduled Monitors. These tasks can also perform routine  maintenance or troubleshooting tasks, like rotating backup revisions or deleting shadow copies. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Maintenance Tasks</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Use this for infrequent Maintenance tasks.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RMM</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -600,7 +695,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Scheduled Tasks</a:t>
+            <a:t>: This should be used for script and task deployment, or</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -612,24 +707,22 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>: Use this for scheduled Monitors.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Maintenance Tasks: Use this for scheduled Maintenance.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t> other one-time tasks.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MITKY</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
@@ -640,33 +733,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>RMM: This should be used for script and task deployment, or</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> other one-time tasks.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>MITKY: This source is available</a:t>
+            <a:t>: This source is available</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -715,50 +782,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Use 1000 block for host or physical server monitoring events.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Use 3000 block for VM monitoring events.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Use 8000 block for Maintenance tasks.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>Use 1000 block for host or physical server monitoring events,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> except for Windows Server Backup.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -780,7 +817,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Group events sequentially:</a:t>
+            <a:t>Use 2000 block for Windows Server</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Backup events or events related to backup revisions created by WSB.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US"/>
@@ -798,12 +847,14 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Use XXX0 to indicate that the setting being checked is not configured.</a:t>
+            <a:t>Use 3000 block for VM monitoring events.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
@@ -814,57 +865,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Use XXX1 for critical events, or the worst-case result. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Use XXX2+ for other errors or warnings.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Use XXX9 for optimal results.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Use subsequent</a:t>
+            <a:t>Use 8000 block for Maintenance tasks</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -876,8 +877,11 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> numbers for additional information.</a:t>
-          </a:r>
+            <a:t> for any server type.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -889,6 +893,114 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Group events sequentially:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use XXX0 to indicate that the setting being checked is not configured.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use XXX1 for critical events, or the worst-case result. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use XXX2+ for other errors or warnings.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use XXX9 for optimal results.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use subsequent</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> numbers for additional information.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -900,6 +1012,17 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
@@ -946,7 +1069,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>in this sheet.</a:t>
+            <a:t>in this sheet. Also confirm if a Datto monitor needs to be created or updated.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1971,7 +2094,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,32 +2103,32 @@
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="H2" s="13"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="2"/>
     </row>
     <row r="29" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J29" s="17"/>
+      <c r="J29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2022,7 +2145,720 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="16" style="20" customWidth="1"/>
+    <col min="4" max="4" width="166.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="33" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>102</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>109</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70440B0E-7E87-4616-B447-BAF53EC0D299}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="166.5703125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>1001</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>1009</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>1060</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>1061</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>1068</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DA6BE0-6D8B-47E8-89E5-07907AFE6D9E}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="166.5703125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2010</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2011</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2012</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>2030</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>2031</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>2032</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>2033</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2034</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>2038</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>2039</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46">
+        <v>2050</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2051</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2054</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>2055</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>2056</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>2057</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>2058</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>2059</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="46">
+        <v>2070</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+    </row>
+    <row r="23" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>2071</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="46">
+        <v>2072</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>2073</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>2074</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>2075</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>2076</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>2079</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D1FCD9-0DC4-4C06-A258-930553BD7C29}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,71 +2871,165 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:6" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
-        <v>102</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="25"/>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <v>109</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="27"/>
+      <c r="E2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2110,617 +3040,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70440B0E-7E87-4616-B447-BAF53EC0D299}">
-  <dimension ref="A1:F27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16" style="8" customWidth="1"/>
-    <col min="4" max="4" width="166.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-    </row>
-    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
-        <v>1000</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
-        <v>1001</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
-        <v>1009</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>1010</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>1011</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>1012</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
-        <v>1019</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <v>1021</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>1022</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>1023</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>1025</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>1026</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>1027</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>1028</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
-        <v>1039</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
-        <v>1050</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="34">
-        <v>1051</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>1052</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="34">
-        <v>1053</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>1054</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="36">
-        <v>1059</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
-        <v>1061</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1068</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="36">
-        <v>1069</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D1FCD9-0DC4-4C06-A258-930553BD7C29}">
-  <dimension ref="A1:F27"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07352D7-56BB-4359-8F7E-BF3E06B00285}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" customWidth="1"/>
-    <col min="4" max="4" width="166.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07352D7-56BB-4359-8F7E-BF3E06B00285}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,178 +3059,34 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="1" spans="1:6" s="44" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>8100</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>8101</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>8102</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>8103</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>8104</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>8109</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>8110</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8130</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8131</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
-        <v>8139</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>48</v>
+      <c r="E2" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update wsb script and excel sheet
</commit_message>
<xml_diff>
--- a/MITKY-CustomEventLogEventIDs.xlsx
+++ b/MITKY-CustomEventLogEventIDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitky0051-my.sharepoint.com/personal/jason_mitky_com/Documents/Documents/GitHub/RMMCustomMonitors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="525" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{340A8F43-24C3-4158-A65D-7C39986D1384}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="13_ncr:1_{C8EBD7CB-E3BC-4093-8543-28367789C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E55D8F96-00A3-4138-AD74-B4E973AD0EFE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{207F7709-C117-4E36-9CC8-F108324BDCB9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>EVENT ID</t>
   </si>
@@ -70,42 +70,15 @@
     <t xml:space="preserve">Hyper-V checkpoints were detected. Check if they are still needed or can be deleted. </t>
   </si>
   <si>
-    <t>Windows Server Backup is not configured for this server.</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
-    <t>The last Windows Server Backup operation reported an error.</t>
-  </si>
-  <si>
-    <t>Could not find a successful Windows Server Backup in the last 24 hours.</t>
-  </si>
-  <si>
-    <t>Windows Server Backup completed successfully within the last 24 hours.</t>
-  </si>
-  <si>
     <t>Critical</t>
   </si>
   <si>
     <t>The backup drive was not found!</t>
   </si>
   <si>
-    <t>There are at least four backup revisions present.</t>
-  </si>
-  <si>
-    <t>There are less than four backup revisions present. Schedule additional revisions.</t>
-  </si>
-  <si>
-    <t>There are less than four backup revisions present. Removing extra files from the backup drive may free enough space for more revisions.</t>
-  </si>
-  <si>
-    <t>There are less than four backup revisions present. The backup drive does not have space for four revisions.</t>
-  </si>
-  <si>
-    <t>There are less than four backup revisions present. There are less than four revisions scheduled. The backup drive does not have space for four revisions.</t>
-  </si>
-  <si>
     <t>External backups are scheduled, but the external backup drive was not found!</t>
   </si>
   <si>
@@ -133,9 +106,6 @@
     <t>YES</t>
   </si>
   <si>
-    <t>Backup revisions could not be checked because of recent backup failures.</t>
-  </si>
-  <si>
     <t>No Virtual Machines were detected or the Get-VM cmdlet failed! Check if Hyper-V is enabled for this server or if VMs should be present.</t>
   </si>
   <si>
@@ -154,15 +124,9 @@
     <t>The last Windows Server Backup revision could not be renamed! Check that the last backup has completed or if another process has the folder or files open.</t>
   </si>
   <si>
-    <t>Not enough drive space for the scheduled number of revisions. The oldest revision was deleted.</t>
-  </si>
-  <si>
     <t>Backup revisions were successfully rotated.</t>
   </si>
   <si>
-    <t>There were less than four backup revisions. An additional revision was scheduled.</t>
-  </si>
-  <si>
     <t>(DO NOT USE) Deleting shadow copies critical event.</t>
   </si>
   <si>
@@ -205,7 +169,10 @@
     <t>There are not enough backup revisions present. Removing other data from the backup drive may free enough space for more revisions.</t>
   </si>
   <si>
-    <t>Failed to delete previous revision: $revName! Check if it is open in another process.</t>
+    <t>Failed to delete previous revision! Check if it is open in another process.</t>
+  </si>
+  <si>
+    <t>Windows Server Backup is not configured for this server or has not run.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +329,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -489,6 +456,13 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2099,7 +2073,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -2154,7 +2128,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="26" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -2176,10 +2150,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2187,16 +2161,16 @@
         <v>102</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F3" s="11"/>
     </row>
@@ -2205,16 +2179,16 @@
         <v>109</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F4" s="13"/>
     </row>
@@ -2248,7 +2222,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2270,10 +2244,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2287,10 +2261,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2333,16 +2307,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2353,10 +2327,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2370,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2390,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DA6BE0-6D8B-47E8-89E5-07907AFE6D9E}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2383,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2431,414 +2405,257 @@
         <v>2</v>
       </c>
       <c r="E2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37">
+        <v>2030</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2031</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="19" t="s">
+    </row>
+    <row r="5" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>2032</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>2010</v>
-      </c>
-      <c r="B3" s="14" t="s">
+    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>2033</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="41" t="s">
+      <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2011</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2012</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>2019</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="44" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
-        <v>2030</v>
+        <v>2034</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>2031</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="54">
+        <v>2035</v>
+      </c>
+      <c r="B8" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>2036</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>2039</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
+        <v>2070</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>2032</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="D11" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>2071</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D12" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37">
+        <v>2072</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
-        <v>2033</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>2073</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>2034</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>2038</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>2039</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="43" t="s">
+      <c r="C14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="44" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
-        <v>2050</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>15</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>2051</v>
-      </c>
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>2074</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>2054</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>2075</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>2055</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="C16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>2076</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>2056</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>2079</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>19</v>
-      </c>
+      <c r="C18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2057</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>2058</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>2059</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37">
-        <v>2070</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-    </row>
-    <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
-        <v>2071</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37">
-        <v>2072</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
-        <v>2073</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
-        <v>2074</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
-        <v>2075</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
-        <v>2076</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>2079</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="41"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2869,7 +2686,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="31" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -2891,10 +2708,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3057,7 +2874,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="35" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -3079,10 +2896,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>